<commit_message>
pdf and import finish
</commit_message>
<xml_diff>
--- a/admin_assets/exel-formate/ADMS_INCREMENT_LETTER.xlsx
+++ b/admin_assets/exel-formate/ADMS_INCREMENT_LETTER.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Enter FFI Employee ID: *</t>
   </si>
@@ -78,35 +78,20 @@
     <t>CTC: *</t>
   </si>
   <si>
-    <t>iyappan</t>
-  </si>
-  <si>
-    <t>iya111</t>
+    <t>fff1616</t>
+  </si>
+  <si>
+    <t>GROFERS INDIA PVT LTD</t>
   </si>
   <si>
     <t>Format 1</t>
-  </si>
-  <si>
-    <t>iya1112</t>
-  </si>
-  <si>
-    <t>iya1113</t>
-  </si>
-  <si>
-    <t>iya1114</t>
-  </si>
-  <si>
-    <t>iya111555555</t>
-  </si>
-  <si>
-    <t>iya34343434</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +114,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -157,10 +148,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,16 +447,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BQ7"/>
+  <dimension ref="A1:BQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
@@ -656,368 +648,64 @@
     </row>
     <row r="2" spans="1:69">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2">
-        <v>435</v>
+        <v>332</v>
       </c>
       <c r="E2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F2">
-        <v>43543</v>
+        <v>43</v>
       </c>
       <c r="G2">
-        <v>5454</v>
+        <v>46</v>
       </c>
       <c r="H2">
-        <v>43543</v>
+        <v>444</v>
       </c>
       <c r="I2">
-        <v>4554</v>
+        <v>345</v>
       </c>
       <c r="J2">
-        <v>566</v>
+        <v>456</v>
       </c>
       <c r="K2">
-        <v>464</v>
+        <v>546554</v>
       </c>
       <c r="L2">
-        <v>465</v>
+        <v>546</v>
       </c>
       <c r="M2">
+        <v>56</v>
+      </c>
+      <c r="N2">
         <v>546</v>
       </c>
-      <c r="N2">
-        <v>654</v>
-      </c>
       <c r="O2">
-        <v>546545</v>
+        <v>45665</v>
       </c>
       <c r="P2">
-        <v>54654</v>
+        <v>45654</v>
       </c>
       <c r="Q2">
-        <v>54654</v>
+        <v>456</v>
       </c>
       <c r="R2">
-        <v>46546</v>
+        <v>456</v>
       </c>
       <c r="S2">
-        <v>6465</v>
+        <v>64</v>
       </c>
       <c r="T2">
-        <v>5654</v>
-      </c>
-    </row>
-    <row r="3" spans="1:69">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3">
-        <v>435</v>
-      </c>
-      <c r="E3">
-        <v>435</v>
-      </c>
-      <c r="F3">
-        <v>43543</v>
-      </c>
-      <c r="G3">
-        <v>5454</v>
-      </c>
-      <c r="H3">
-        <v>43543</v>
-      </c>
-      <c r="I3">
-        <v>4554</v>
-      </c>
-      <c r="J3">
-        <v>566</v>
-      </c>
-      <c r="K3">
-        <v>464</v>
-      </c>
-      <c r="L3">
-        <v>465</v>
-      </c>
-      <c r="M3">
-        <v>546</v>
-      </c>
-      <c r="N3">
-        <v>654</v>
-      </c>
-      <c r="O3">
-        <v>546545</v>
-      </c>
-      <c r="P3">
-        <v>54654</v>
-      </c>
-      <c r="Q3">
-        <v>54654</v>
-      </c>
-      <c r="R3">
-        <v>46546</v>
-      </c>
-      <c r="S3">
-        <v>6465</v>
-      </c>
-      <c r="T3">
-        <v>5654</v>
-      </c>
-    </row>
-    <row r="4" spans="1:69">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4">
-        <v>435</v>
-      </c>
-      <c r="E4">
-        <v>435</v>
-      </c>
-      <c r="F4">
-        <v>43543</v>
-      </c>
-      <c r="G4">
-        <v>5454</v>
-      </c>
-      <c r="H4">
-        <v>43543</v>
-      </c>
-      <c r="I4">
-        <v>4554</v>
-      </c>
-      <c r="J4">
-        <v>566</v>
-      </c>
-      <c r="K4">
-        <v>464</v>
-      </c>
-      <c r="L4">
-        <v>465</v>
-      </c>
-      <c r="M4">
-        <v>546</v>
-      </c>
-      <c r="N4">
-        <v>654</v>
-      </c>
-      <c r="O4">
-        <v>546545</v>
-      </c>
-      <c r="P4">
-        <v>54654</v>
-      </c>
-      <c r="Q4">
-        <v>54654</v>
-      </c>
-      <c r="R4">
-        <v>46546</v>
-      </c>
-      <c r="S4">
-        <v>6465</v>
-      </c>
-      <c r="T4">
-        <v>5654</v>
-      </c>
-    </row>
-    <row r="5" spans="1:69">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5">
-        <v>435</v>
-      </c>
-      <c r="E5">
-        <v>435</v>
-      </c>
-      <c r="F5">
-        <v>43543</v>
-      </c>
-      <c r="G5">
-        <v>5454</v>
-      </c>
-      <c r="H5">
-        <v>43543</v>
-      </c>
-      <c r="I5">
-        <v>4554</v>
-      </c>
-      <c r="J5">
-        <v>566</v>
-      </c>
-      <c r="K5">
-        <v>464</v>
-      </c>
-      <c r="L5">
-        <v>465</v>
-      </c>
-      <c r="M5">
-        <v>546</v>
-      </c>
-      <c r="N5">
-        <v>654</v>
-      </c>
-      <c r="O5">
-        <v>546545</v>
-      </c>
-      <c r="P5">
-        <v>54654</v>
-      </c>
-      <c r="Q5">
-        <v>54654</v>
-      </c>
-      <c r="R5">
-        <v>46546</v>
-      </c>
-      <c r="S5">
-        <v>6465</v>
-      </c>
-      <c r="T5">
-        <v>5654</v>
-      </c>
-    </row>
-    <row r="6" spans="1:69">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>435</v>
-      </c>
-      <c r="E6">
-        <v>435</v>
-      </c>
-      <c r="F6">
-        <v>43543</v>
-      </c>
-      <c r="G6">
-        <v>5454</v>
-      </c>
-      <c r="H6">
-        <v>43543</v>
-      </c>
-      <c r="I6">
-        <v>4554</v>
-      </c>
-      <c r="J6">
-        <v>566</v>
-      </c>
-      <c r="K6">
-        <v>464</v>
-      </c>
-      <c r="L6">
-        <v>465</v>
-      </c>
-      <c r="M6">
-        <v>546</v>
-      </c>
-      <c r="N6">
-        <v>654</v>
-      </c>
-      <c r="O6">
-        <v>546545</v>
-      </c>
-      <c r="P6">
-        <v>54654</v>
-      </c>
-      <c r="Q6">
-        <v>54654</v>
-      </c>
-      <c r="R6">
-        <v>46546</v>
-      </c>
-      <c r="S6">
-        <v>6465</v>
-      </c>
-      <c r="T6">
-        <v>5654</v>
-      </c>
-    </row>
-    <row r="7" spans="1:69">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7">
-        <v>435</v>
-      </c>
-      <c r="E7">
-        <v>435</v>
-      </c>
-      <c r="F7">
-        <v>43543</v>
-      </c>
-      <c r="G7">
-        <v>5454</v>
-      </c>
-      <c r="H7">
-        <v>43543</v>
-      </c>
-      <c r="I7">
-        <v>4554</v>
-      </c>
-      <c r="J7">
-        <v>566</v>
-      </c>
-      <c r="K7">
-        <v>464</v>
-      </c>
-      <c r="L7">
-        <v>465</v>
-      </c>
-      <c r="M7">
-        <v>546</v>
-      </c>
-      <c r="N7">
-        <v>654</v>
-      </c>
-      <c r="O7">
-        <v>546545</v>
-      </c>
-      <c r="P7">
-        <v>54654</v>
-      </c>
-      <c r="Q7">
-        <v>54654</v>
-      </c>
-      <c r="R7">
-        <v>46546</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to dcs approval d_table by madhu
</commit_message>
<xml_diff>
--- a/admin_assets/exel-formate/ADMS_INCREMENT_LETTER.xlsx
+++ b/admin_assets/exel-formate/ADMS_INCREMENT_LETTER.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Wbo_fretusfolks\admin_assets\exel-formate\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358C39EA-FCDA-4484-971D-4BB238AC04F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="60" windowWidth="20730" windowHeight="9510"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,20 +84,20 @@
     <t>CTC: *</t>
   </si>
   <si>
-    <t>fff1616</t>
-  </si>
-  <si>
     <t>GROFERS INDIA PVT LTD</t>
   </si>
   <si>
     <t>Format 1</t>
+  </si>
+  <si>
+    <t>FFI1311</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +165,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -205,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -237,9 +251,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -271,6 +303,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,96 +496,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BQ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" activeCellId="1" sqref="A2 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" customWidth="1"/>
-    <col min="18" max="18" width="18.140625" customWidth="1"/>
-    <col min="19" max="19" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="14" max="14" width="7.5546875" customWidth="1"/>
+    <col min="15" max="15" width="20.109375" customWidth="1"/>
+    <col min="16" max="16" width="21.6640625" customWidth="1"/>
+    <col min="17" max="17" width="19.109375" customWidth="1"/>
+    <col min="18" max="18" width="18.109375" customWidth="1"/>
+    <col min="19" max="19" width="21.44140625" customWidth="1"/>
     <col min="20" max="20" width="9" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" customWidth="1"/>
-    <col min="22" max="22" width="16.5703125" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" customWidth="1"/>
+    <col min="22" max="22" width="16.5546875" customWidth="1"/>
     <col min="23" max="23" width="19" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" customWidth="1"/>
-    <col min="25" max="25" width="17.5703125" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" customWidth="1"/>
+    <col min="25" max="25" width="17.5546875" customWidth="1"/>
     <col min="26" max="26" width="22" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" customWidth="1"/>
-    <col min="28" max="28" width="16.140625" customWidth="1"/>
-    <col min="29" max="29" width="22.28515625" customWidth="1"/>
-    <col min="30" max="30" width="7.5703125" customWidth="1"/>
-    <col min="31" max="31" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.88671875" customWidth="1"/>
+    <col min="28" max="28" width="16.109375" customWidth="1"/>
+    <col min="29" max="29" width="22.33203125" customWidth="1"/>
+    <col min="30" max="30" width="7.5546875" customWidth="1"/>
+    <col min="31" max="31" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="19" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="21" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="20" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="8" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="6" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="23" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="20" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" s="2" customFormat="1">
+    <row r="1" spans="1:69" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,15 +696,15 @@
       <c r="BP1"/>
       <c r="BQ1"/>
     </row>
-    <row r="2" spans="1:69">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
       </c>
       <c r="D2">
         <v>332</v>
@@ -715,24 +765,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
complete increment letter process by iyappan
</commit_message>
<xml_diff>
--- a/admin_assets/exel-formate/ADMS_INCREMENT_LETTER.xlsx
+++ b/admin_assets/exel-formate/ADMS_INCREMENT_LETTER.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Enter FFI Employee ID: *</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Client Company Name: *</t>
   </si>
   <si>
-    <t>Offer Letter For: *</t>
-  </si>
-  <si>
     <t>Other Allowance: *</t>
   </si>
   <si>
@@ -81,7 +78,7 @@
     <t>Client Id: *</t>
   </si>
   <si>
-    <t>Format Id:*</t>
+    <t>Effective Date: *</t>
   </si>
 </sst>
 </file>
@@ -452,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BQ2"/>
+  <dimension ref="A1:BP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -467,7 +464,7 @@
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" customWidth="1"/>
@@ -540,7 +537,7 @@
     <col min="78" max="78" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" s="2" customFormat="1">
+    <row r="1" spans="1:68" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +545,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -569,7 +566,7 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>7</v>
@@ -599,15 +596,13 @@
         <v>15</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U1"/>
       <c r="V1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="W1"/>
       <c r="X1"/>
       <c r="Y1"/>
       <c r="Z1"/>
@@ -653,9 +648,8 @@
       <c r="BN1"/>
       <c r="BO1"/>
       <c r="BP1"/>
-      <c r="BQ1"/>
     </row>
-    <row r="2" spans="1:69">
+    <row r="2" spans="1:68">
       <c r="B2" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increment letter by iyappan
</commit_message>
<xml_diff>
--- a/admin_assets/exel-formate/ADMS_INCREMENT_LETTER.xlsx
+++ b/admin_assets/exel-formate/ADMS_INCREMENT_LETTER.xlsx
@@ -452,89 +452,88 @@
   <dimension ref="A1:BP2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" customWidth="1"/>
-    <col min="16" max="16" width="21.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" customWidth="1"/>
-    <col min="18" max="18" width="18.140625" customWidth="1"/>
-    <col min="19" max="19" width="21.42578125" customWidth="1"/>
-    <col min="20" max="20" width="9" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" customWidth="1"/>
-    <col min="22" max="22" width="16.5703125" customWidth="1"/>
-    <col min="23" max="23" width="19" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" customWidth="1"/>
-    <col min="25" max="25" width="17.5703125" customWidth="1"/>
-    <col min="26" max="26" width="22" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" customWidth="1"/>
-    <col min="28" max="28" width="16.140625" customWidth="1"/>
-    <col min="29" max="29" width="22.28515625" customWidth="1"/>
-    <col min="30" max="30" width="7.5703125" customWidth="1"/>
-    <col min="31" max="31" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="22" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="20" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="6" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="23" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="20" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" customWidth="1"/>
+    <col min="17" max="17" width="18.140625" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" customWidth="1"/>
+    <col min="19" max="19" width="9" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" customWidth="1"/>
+    <col min="22" max="22" width="19" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" customWidth="1"/>
+    <col min="24" max="24" width="17.5703125" customWidth="1"/>
+    <col min="25" max="25" width="22" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" customWidth="1"/>
+    <col min="27" max="27" width="16.140625" customWidth="1"/>
+    <col min="28" max="28" width="22.28515625" customWidth="1"/>
+    <col min="29" max="29" width="7.5703125" customWidth="1"/>
+    <col min="30" max="30" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="22" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="21" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="8" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="6" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="20" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:68" s="2" customFormat="1">
@@ -545,58 +544,58 @@
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="U1"/>
       <c r="V1" s="1" t="s">

</xml_diff>